<commit_message>
better houses and regions
</commit_message>
<xml_diff>
--- a/Got.xlsx
+++ b/Got.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="108">
   <si>
     <t>House</t>
   </si>
@@ -104,48 +104,12 @@
     <t>Westerose</t>
   </si>
   <si>
-    <t>The fingers</t>
-  </si>
-  <si>
-    <t>The Trident</t>
-  </si>
-  <si>
-    <t>Kings Landing</t>
-  </si>
-  <si>
-    <t>Dragonstone</t>
-  </si>
-  <si>
-    <t>The Center</t>
-  </si>
-  <si>
     <t>Esos</t>
   </si>
   <si>
-    <t>The South</t>
-  </si>
-  <si>
     <t>Horn Hill</t>
   </si>
   <si>
-    <t>Sandstone</t>
-  </si>
-  <si>
-    <t>Three Towers</t>
-  </si>
-  <si>
-    <t>Rainwood</t>
-  </si>
-  <si>
-    <t>Pike</t>
-  </si>
-  <si>
-    <t>The Twins</t>
-  </si>
-  <si>
-    <t>The Eyrie</t>
-  </si>
-  <si>
     <t>Male</t>
   </si>
   <si>
@@ -261,13 +225,136 @@
   </si>
   <si>
     <t>LocationX</t>
+  </si>
+  <si>
+    <t>The Vale</t>
+  </si>
+  <si>
+    <t>The Riverlands</t>
+  </si>
+  <si>
+    <t>Tully </t>
+  </si>
+  <si>
+    <t>Riverrun</t>
+  </si>
+  <si>
+    <t>Arryn </t>
+  </si>
+  <si>
+    <t>Eyrie</t>
+  </si>
+  <si>
+    <t>The Westernlands</t>
+  </si>
+  <si>
+    <t>Casterly Rock</t>
+  </si>
+  <si>
+    <t>Storm's End</t>
+  </si>
+  <si>
+    <t>The Stormlands</t>
+  </si>
+  <si>
+    <t>The Reach</t>
+  </si>
+  <si>
+    <t>Tyrell </t>
+  </si>
+  <si>
+    <t>Highgarden</t>
+  </si>
+  <si>
+    <t>Martell </t>
+  </si>
+  <si>
+    <t>Sunspear</t>
+  </si>
+  <si>
+    <t>Dorne</t>
+  </si>
+  <si>
+    <t>Pyke</t>
+  </si>
+  <si>
+    <t>Iron Islands</t>
+  </si>
+  <si>
+    <t>Acorn Hall</t>
+  </si>
+  <si>
+    <t>Wayfarer's Rest</t>
+  </si>
+  <si>
+    <t>The Bloody Gate</t>
+  </si>
+  <si>
+    <t>Redfort</t>
+  </si>
+  <si>
+    <t>Strongsong</t>
+  </si>
+  <si>
+    <t>Lannisport</t>
+  </si>
+  <si>
+    <t>Feastfires</t>
+  </si>
+  <si>
+    <t>Kayce</t>
+  </si>
+  <si>
+    <t>Claegane Hall</t>
+  </si>
+  <si>
+    <t>Evenfall Hall</t>
+  </si>
+  <si>
+    <t>Tarth</t>
+  </si>
+  <si>
+    <t>Crow's nest</t>
+  </si>
+  <si>
+    <t>Old Oak</t>
+  </si>
+  <si>
+    <t>Cider Hall</t>
+  </si>
+  <si>
+    <t>Wyl</t>
+  </si>
+  <si>
+    <t>Lemonwood</t>
+  </si>
+  <si>
+    <t>Godsgrace</t>
+  </si>
+  <si>
+    <t>Vaith</t>
+  </si>
+  <si>
+    <t>The Tor</t>
+  </si>
+  <si>
+    <t>Naggas Rib</t>
+  </si>
+  <si>
+    <t>Hammerhorn</t>
+  </si>
+  <si>
+    <t>Ten Towers</t>
+  </si>
+  <si>
+    <t>Balish Keep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +371,12 @@
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Georgia"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -307,9 +400,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -591,10 +685,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31:J47"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -602,7 +696,7 @@
     <col min="5" max="5" width="19.375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.375" customWidth="1"/>
+    <col min="8" max="8" width="24.25" customWidth="1"/>
     <col min="9" max="9" width="12.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12.375" customWidth="1"/>
   </cols>
@@ -615,10 +709,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -627,13 +721,13 @@
         <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="H1" t="s">
         <v>5</v>
       </c>
       <c r="I1" t="s">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="J1" t="s">
         <v>3</v>
@@ -656,10 +750,10 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D2" t="str">
         <f>C2&amp;";"&amp;B2</f>
@@ -686,7 +780,7 @@
         <v>The Wall;The North;Westerose</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
@@ -694,10 +788,10 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D3" t="str">
         <f t="shared" ref="D3:D47" si="0">C3&amp;";"&amp;B3</f>
@@ -713,18 +807,18 @@
         <v>19</v>
       </c>
       <c r="H3" t="str">
-        <f t="shared" ref="H3:H47" si="1">G3&amp;";"&amp;F3</f>
+        <f t="shared" ref="H3:H36" si="1">G3&amp;";"&amp;F3</f>
         <v>The North;Westerose</v>
       </c>
       <c r="I3" t="s">
         <v>21</v>
       </c>
       <c r="J3" t="str">
-        <f t="shared" ref="J3:J47" si="2">I3&amp;";"&amp;H3</f>
+        <f t="shared" ref="J3:J36" si="2">I3&amp;";"&amp;H3</f>
         <v>Winterfell;The North;Westerose</v>
       </c>
       <c r="K3" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
@@ -732,10 +826,10 @@
         <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D4" t="str">
         <f t="shared" si="0"/>
@@ -767,10 +861,10 @@
         <v>17</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C5" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D5" t="str">
         <f t="shared" si="0"/>
@@ -802,10 +896,10 @@
         <v>18</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D6" t="str">
         <f t="shared" si="0"/>
@@ -817,120 +911,129 @@
       <c r="F6" t="s">
         <v>25</v>
       </c>
-      <c r="G6" t="s">
-        <v>30</v>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
       </c>
       <c r="H6" t="str">
         <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
-      </c>
-      <c r="I6" t="s">
-        <v>26</v>
+        <v>The Riverlands;Westerose</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>70</v>
       </c>
       <c r="J6" t="str">
         <f t="shared" si="2"/>
-        <v>The fingers;The Center;Westerose</v>
+        <v>Riverrun;The Riverlands;Westerose</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>56</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 6;Season 1</v>
+      </c>
+      <c r="E7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="1"/>
+        <v>The Riverlands;Westerose</v>
+      </c>
+      <c r="I7" t="s">
+        <v>85</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="2"/>
+        <v>Acorn Hall;The Riverlands;Westerose</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
         <v>42</v>
       </c>
-      <c r="C7" t="s">
-        <v>53</v>
-      </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 6;Season 1</v>
-      </c>
-      <c r="E7" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
+      <c r="D8" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 7;Season 1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="1"/>
+        <v>The Riverlands;Westerose</v>
+      </c>
+      <c r="I8" t="s">
+        <v>86</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="2"/>
+        <v>Wayfarer's Rest;The Riverlands;Westerose</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="str">
-        <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
-      </c>
-      <c r="I7" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" t="str">
-        <f t="shared" si="2"/>
-        <v>The Trident;The Center;Westerose</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" t="s">
-        <v>54</v>
-      </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 7;Season 1</v>
-      </c>
-      <c r="F8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G8" t="s">
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 8;Season 1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="1"/>
+        <v>The Vale;Westerose</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="2"/>
+        <v>Eyrie;The Vale;Westerose</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
         <v>30</v>
       </c>
-      <c r="H8" t="str">
-        <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
-      </c>
-      <c r="I8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" t="str">
-        <f t="shared" si="2"/>
-        <v>Kings Landing;The Center;Westerose</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C9" t="s">
-        <v>55</v>
-      </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 8;Season 1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>25</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="str">
-        <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
-      </c>
-      <c r="J9" t="str">
-        <f t="shared" si="2"/>
-        <v>Dragonstone;The Center;Westerose</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
-        <v>42</v>
-      </c>
       <c r="C10" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D10" t="str">
         <f t="shared" si="0"/>
@@ -939,27 +1042,30 @@
       <c r="F10" t="s">
         <v>25</v>
       </c>
-      <c r="G10" t="s">
-        <v>30</v>
+      <c r="G10" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H10" t="str">
         <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
+        <v>The Vale;Westerose</v>
       </c>
       <c r="I10" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="J10" t="str">
         <f t="shared" si="2"/>
-        <v>Pike;The Center;Westerose</v>
+        <v>The Bloody Gate;The Vale;Westerose</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>80</v>
+      </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D11" t="str">
         <f t="shared" si="0"/>
@@ -968,27 +1074,27 @@
       <c r="F11" t="s">
         <v>25</v>
       </c>
-      <c r="G11" t="s">
-        <v>30</v>
+      <c r="G11" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H11" t="str">
         <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
+        <v>The Vale;Westerose</v>
       </c>
       <c r="I11" t="s">
-        <v>38</v>
+        <v>88</v>
       </c>
       <c r="J11" t="str">
         <f t="shared" si="2"/>
-        <v>The Twins;The Center;Westerose</v>
+        <v>Redfort;The Vale;Westerose</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D12" t="str">
         <f t="shared" si="0"/>
@@ -997,27 +1103,28 @@
       <c r="F12" t="s">
         <v>25</v>
       </c>
-      <c r="G12" t="s">
-        <v>30</v>
+      <c r="G12" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H12" t="str">
         <f t="shared" si="1"/>
-        <v>The Center;Westerose</v>
+        <v>The Vale;Westerose</v>
       </c>
       <c r="I12" t="s">
-        <v>39</v>
+        <v>89</v>
       </c>
       <c r="J12" t="str">
         <f t="shared" si="2"/>
-        <v>The Eyrie;The Center;Westerose</v>
+        <v>Strongsong;The Vale;Westerose</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A13" s="2"/>
       <c r="B13" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D13" t="str">
         <f t="shared" si="0"/>
@@ -1026,27 +1133,27 @@
       <c r="F13" t="s">
         <v>25</v>
       </c>
-      <c r="G13" t="s">
-        <v>32</v>
+      <c r="G13" s="2" t="s">
+        <v>67</v>
       </c>
       <c r="H13" t="str">
         <f t="shared" si="1"/>
-        <v>The South;Westerose</v>
+        <v>The Vale;Westerose</v>
       </c>
       <c r="I13" t="s">
-        <v>33</v>
+        <v>107</v>
       </c>
       <c r="J13" t="str">
         <f t="shared" si="2"/>
-        <v>Horn Hill;The South;Westerose</v>
+        <v>Balish Keep;The Vale;Westerose</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C14" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D14" t="str">
         <f t="shared" si="0"/>
@@ -1055,27 +1162,27 @@
       <c r="F14" t="s">
         <v>25</v>
       </c>
-      <c r="G14" t="s">
-        <v>32</v>
+      <c r="G14" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H14" t="str">
         <f t="shared" si="1"/>
-        <v>The South;Westerose</v>
-      </c>
-      <c r="I14" t="s">
-        <v>34</v>
+        <v>The Westernlands;Westerose</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>74</v>
       </c>
       <c r="J14" t="str">
         <f t="shared" si="2"/>
-        <v>Sandstone;The South;Westerose</v>
+        <v>Casterly Rock;The Westernlands;Westerose</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D15" t="str">
         <f t="shared" si="0"/>
@@ -1084,27 +1191,27 @@
       <c r="F15" t="s">
         <v>25</v>
       </c>
-      <c r="G15" t="s">
-        <v>32</v>
+      <c r="G15" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H15" t="str">
         <f t="shared" si="1"/>
-        <v>The South;Westerose</v>
+        <v>The Westernlands;Westerose</v>
       </c>
       <c r="I15" t="s">
-        <v>35</v>
+        <v>90</v>
       </c>
       <c r="J15" t="str">
         <f t="shared" si="2"/>
-        <v>Three Towers;The South;Westerose</v>
+        <v>Lannisport;The Westernlands;Westerose</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D16" t="str">
         <f t="shared" si="0"/>
@@ -1113,629 +1220,975 @@
       <c r="F16" t="s">
         <v>25</v>
       </c>
-      <c r="G16" t="s">
-        <v>32</v>
+      <c r="G16" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H16" t="str">
         <f t="shared" si="1"/>
-        <v>The South;Westerose</v>
+        <v>The Westernlands;Westerose</v>
       </c>
       <c r="I16" t="s">
-        <v>36</v>
+        <v>91</v>
       </c>
       <c r="J16" t="str">
         <f t="shared" si="2"/>
-        <v>Rainwood;The South;Westerose</v>
+        <v>Feastfires;The Westernlands;Westerose</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D17" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 7;Season 2</v>
       </c>
       <c r="F17" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H17" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
+        <v>The Westernlands;Westerose</v>
       </c>
       <c r="I17" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
       <c r="J17" t="str">
         <f t="shared" si="2"/>
-        <v>Myr;The East;Esos</v>
+        <v>Kayce;The Westernlands;Westerose</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
         <v>43</v>
       </c>
-      <c r="C18" t="s">
-        <v>55</v>
-      </c>
       <c r="D18" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 8;Season 2</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
-      </c>
-      <c r="G18" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>73</v>
       </c>
       <c r="H18" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
+        <v>The Westernlands;Westerose</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="J18" t="str">
         <f t="shared" si="2"/>
-        <v>Tyros;The East;Esos</v>
+        <v>Claegane Hall;The Westernlands;Westerose</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D19" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 9;Season 2</v>
       </c>
       <c r="F19" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="H19" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
-      </c>
-      <c r="I19" t="s">
-        <v>62</v>
+        <v>The Stormlands;Westerose</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="J19" t="str">
         <f t="shared" si="2"/>
-        <v>Lys;The East;Esos</v>
+        <v>Storm's End;The Stormlands;Westerose</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C20" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D20" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 1;Season 3</v>
       </c>
       <c r="F20" t="s">
-        <v>31</v>
-      </c>
-      <c r="G20" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="H20" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
+        <v>The Stormlands;Westerose</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="J20" t="str">
         <f t="shared" si="2"/>
-        <v>Volantis;The East;Esos</v>
+        <v>Evenfall Hall;The Stormlands;Westerose</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C21" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D21" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 2;Season 3</v>
       </c>
       <c r="F21" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="H21" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
+        <v>The Stormlands;Westerose</v>
       </c>
       <c r="I21" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="J21" t="str">
         <f t="shared" si="2"/>
-        <v>Pentos;The East;Esos</v>
+        <v>Tarth;The Stormlands;Westerose</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C22" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D22" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 3;Season 3</v>
       </c>
       <c r="F22" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" t="s">
-        <v>59</v>
+        <v>25</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="H22" t="str">
         <f t="shared" si="1"/>
-        <v>The East;Esos</v>
+        <v>The Stormlands;Westerose</v>
       </c>
       <c r="I22" t="s">
-        <v>65</v>
+        <v>96</v>
       </c>
       <c r="J22" t="str">
         <f t="shared" si="2"/>
-        <v>Braavos;The East;Esos</v>
+        <v>Crow's nest;The Stormlands;Westerose</v>
       </c>
     </row>
     <row r="23" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C23" t="s">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="D23" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 4;Season 3</v>
       </c>
       <c r="F23" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="H23" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
-      </c>
-      <c r="I23" t="s">
-        <v>67</v>
+        <v>The Reach;Westerose</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>79</v>
       </c>
       <c r="J23" t="str">
         <f t="shared" si="2"/>
-        <v>The Dothraki Sea;The West;Esos</v>
+        <v>Highgarden;The Reach;Westerose</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="D24" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 5;Season 3</v>
       </c>
       <c r="F24" t="s">
-        <v>31</v>
-      </c>
-      <c r="G24" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="H24" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>The Reach;Westerose</v>
       </c>
       <c r="I24" t="s">
-        <v>68</v>
+        <v>97</v>
       </c>
       <c r="J24" t="str">
         <f t="shared" si="2"/>
-        <v>Qohor;The West;Esos</v>
+        <v>Old Oak;The Reach;Westerose</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="D25" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 6;Season 3</v>
       </c>
       <c r="F25" t="s">
-        <v>31</v>
-      </c>
-      <c r="G25" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="H25" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>The Reach;Westerose</v>
       </c>
       <c r="I25" t="s">
-        <v>69</v>
+        <v>98</v>
       </c>
       <c r="J25" t="str">
         <f t="shared" si="2"/>
-        <v>The Sorrow;The West;Esos</v>
+        <v>Cider Hall;The Reach;Westerose</v>
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B26" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C26" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="D26" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 7;Season 3</v>
       </c>
       <c r="F26" t="s">
-        <v>31</v>
-      </c>
-      <c r="G26" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>77</v>
       </c>
       <c r="H26" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>The Reach;Westerose</v>
       </c>
       <c r="I26" t="s">
-        <v>70</v>
+        <v>27</v>
       </c>
       <c r="J26" t="str">
         <f t="shared" si="2"/>
-        <v>Mantarys;The West;Esos</v>
+        <v>Horn Hill;The Reach;Westerose</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="D27" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 8;Season 3</v>
       </c>
       <c r="F27" t="s">
-        <v>31</v>
-      </c>
-      <c r="G27" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="H27" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
-      </c>
-      <c r="I27" t="s">
-        <v>71</v>
+        <v>Dorne;Westerose</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="J27" t="str">
         <f t="shared" si="2"/>
-        <v>Astapor;The West;Esos</v>
+        <v>Sunspear;Dorne;Westerose</v>
       </c>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="D28" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 9;Season 3</v>
       </c>
       <c r="F28" t="s">
-        <v>31</v>
-      </c>
-      <c r="G28" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="H28" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>Dorne;Westerose</v>
       </c>
       <c r="I28" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="J28" t="str">
         <f t="shared" si="2"/>
-        <v>Vaes Dothrak;The West;Esos</v>
+        <v>Wyl;Dorne;Westerose</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="D29" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 1;Season 4</v>
       </c>
       <c r="F29" t="s">
-        <v>31</v>
-      </c>
-      <c r="G29" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="H29" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>Dorne;Westerose</v>
       </c>
       <c r="I29" t="s">
-        <v>73</v>
+        <v>100</v>
       </c>
       <c r="J29" t="str">
         <f t="shared" si="2"/>
-        <v>Yunkai;The West;Esos</v>
+        <v>Lemonwood;Dorne;Westerose</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="D30" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 2;Season 4</v>
       </c>
       <c r="F30" t="s">
-        <v>31</v>
-      </c>
-      <c r="G30" t="s">
-        <v>66</v>
+        <v>25</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>82</v>
       </c>
       <c r="H30" t="str">
         <f t="shared" si="1"/>
-        <v>The West;Esos</v>
+        <v>Dorne;Westerose</v>
       </c>
       <c r="I30" t="s">
-        <v>74</v>
+        <v>101</v>
       </c>
       <c r="J30" t="str">
         <f t="shared" si="2"/>
-        <v>Meereen;The West;Esos</v>
+        <v>Godsgrace;Dorne;Westerose</v>
       </c>
     </row>
     <row r="31" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C31" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="D31" t="str">
         <f t="shared" si="0"/>
         <v>Cahpter 3;Season 4</v>
+      </c>
+      <c r="F31" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H31" t="str">
+        <f t="shared" si="1"/>
+        <v>Dorne;Westerose</v>
+      </c>
+      <c r="I31" t="s">
+        <v>102</v>
+      </c>
+      <c r="J31" t="str">
+        <f t="shared" si="2"/>
+        <v>Vaith;Dorne;Westerose</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
+        <v>39</v>
+      </c>
+      <c r="D32" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 4;Season 4</v>
+      </c>
+      <c r="F32" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H32" t="str">
+        <f t="shared" si="1"/>
+        <v>Dorne;Westerose</v>
+      </c>
+      <c r="I32" t="s">
+        <v>103</v>
+      </c>
+      <c r="J32" t="str">
+        <f t="shared" si="2"/>
+        <v>The Tor;Dorne;Westerose</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" t="s">
+        <v>40</v>
+      </c>
+      <c r="D33" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 5;Season 4</v>
+      </c>
+      <c r="F33" t="s">
+        <v>44</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H33" t="str">
+        <f t="shared" si="1"/>
+        <v>Iron Islands;Other</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="J33" t="str">
+        <f t="shared" si="2"/>
+        <v>Pyke;Iron Islands;Other</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 6;Season 4</v>
+      </c>
+      <c r="F34" t="s">
+        <v>44</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H34" t="str">
+        <f t="shared" si="1"/>
+        <v>Iron Islands;Other</v>
+      </c>
+      <c r="I34" t="s">
+        <v>104</v>
+      </c>
+      <c r="J34" t="str">
+        <f t="shared" si="2"/>
+        <v>Naggas Rib;Iron Islands;Other</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>33</v>
+      </c>
+      <c r="C35" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 7;Season 4</v>
+      </c>
+      <c r="F35" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H35" t="str">
+        <f t="shared" si="1"/>
+        <v>Iron Islands;Other</v>
+      </c>
+      <c r="I35" t="s">
+        <v>105</v>
+      </c>
+      <c r="J35" t="str">
+        <f t="shared" si="2"/>
+        <v>Hammerhorn;Iron Islands;Other</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" t="s">
+        <v>43</v>
+      </c>
+      <c r="D36" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 8;Season 4</v>
+      </c>
+      <c r="F36" t="s">
+        <v>44</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="H36" t="str">
+        <f t="shared" si="1"/>
+        <v>Iron Islands;Other</v>
+      </c>
+      <c r="I36" t="s">
+        <v>106</v>
+      </c>
+      <c r="J36" t="str">
+        <f t="shared" si="2"/>
+        <v>Ten Towers;Iron Islands;Other</v>
+      </c>
+    </row>
+    <row r="37" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" t="s">
+        <v>35</v>
+      </c>
+      <c r="D37" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 9;Season 4</v>
+      </c>
+      <c r="F37" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" t="s">
+        <v>47</v>
+      </c>
+      <c r="H37" t="str">
+        <f>G37&amp;";"&amp;F37</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I37" t="s">
+        <v>48</v>
+      </c>
+      <c r="J37" t="str">
+        <f>I37&amp;";"&amp;H37</f>
+        <v>Myr;The East;Esos</v>
+      </c>
+    </row>
+    <row r="38" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B38" t="s">
+        <v>34</v>
+      </c>
+      <c r="C38" t="s">
+        <v>36</v>
+      </c>
+      <c r="D38" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 1;Season 5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>26</v>
+      </c>
+      <c r="G38" t="s">
+        <v>47</v>
+      </c>
+      <c r="H38" t="str">
+        <f>G38&amp;";"&amp;F38</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I38" t="s">
+        <v>49</v>
+      </c>
+      <c r="J38" t="str">
+        <f>I38&amp;";"&amp;H38</f>
+        <v>Tyros;The East;Esos</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" t="s">
+        <v>37</v>
+      </c>
+      <c r="D39" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 2;Season 5</v>
+      </c>
+      <c r="F39" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" t="s">
+        <v>47</v>
+      </c>
+      <c r="H39" t="str">
+        <f>G39&amp;";"&amp;F39</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I39" t="s">
+        <v>50</v>
+      </c>
+      <c r="J39" t="str">
+        <f>I39&amp;";"&amp;H39</f>
+        <v>Lys;The East;Esos</v>
+      </c>
+    </row>
+    <row r="40" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B40" t="s">
+        <v>34</v>
+      </c>
+      <c r="C40" t="s">
+        <v>38</v>
+      </c>
+      <c r="D40" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 3;Season 5</v>
+      </c>
+      <c r="F40" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" t="s">
+        <v>47</v>
+      </c>
+      <c r="H40" t="str">
+        <f>G40&amp;";"&amp;F40</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I40" t="s">
         <v>51</v>
       </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 4;Season 4</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B33" t="s">
-        <v>45</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="J40" t="str">
+        <f>I40&amp;";"&amp;H40</f>
+        <v>Volantis;The East;Esos</v>
+      </c>
+    </row>
+    <row r="41" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B41" t="s">
+        <v>34</v>
+      </c>
+      <c r="C41" t="s">
+        <v>39</v>
+      </c>
+      <c r="D41" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 4;Season 5</v>
+      </c>
+      <c r="F41" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H41" t="str">
+        <f>G41&amp;";"&amp;F41</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I41" t="s">
         <v>52</v>
       </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 5;Season 4</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B34" t="s">
-        <v>45</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="J41" t="str">
+        <f>I41&amp;";"&amp;H41</f>
+        <v>Pentos;The East;Esos</v>
+      </c>
+    </row>
+    <row r="42" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B42" t="s">
+        <v>34</v>
+      </c>
+      <c r="C42" t="s">
+        <v>40</v>
+      </c>
+      <c r="D42" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 5;Season 5</v>
+      </c>
+      <c r="F42" t="s">
+        <v>26</v>
+      </c>
+      <c r="G42" t="s">
+        <v>47</v>
+      </c>
+      <c r="H42" t="str">
+        <f>G42&amp;";"&amp;F42</f>
+        <v>The East;Esos</v>
+      </c>
+      <c r="I42" t="s">
         <v>53</v>
       </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 6;Season 4</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B35" t="s">
-        <v>45</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="J42" t="str">
+        <f>I42&amp;";"&amp;H42</f>
+        <v>Braavos;The East;Esos</v>
+      </c>
+    </row>
+    <row r="43" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B43" t="s">
+        <v>34</v>
+      </c>
+      <c r="C43" t="s">
+        <v>41</v>
+      </c>
+      <c r="D43" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 6;Season 5</v>
+      </c>
+      <c r="F43" t="s">
+        <v>26</v>
+      </c>
+      <c r="G43" t="s">
         <v>54</v>
       </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 7;Season 4</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B36" t="s">
-        <v>45</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="H43" t="str">
+        <f>G43&amp;";"&amp;F43</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I43" t="s">
         <v>55</v>
       </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 8;Season 4</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B37" t="s">
-        <v>45</v>
-      </c>
-      <c r="C37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 9;Season 4</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B38" t="s">
+      <c r="J43" t="str">
+        <f>I43&amp;";"&amp;H43</f>
+        <v>The Dothraki Sea;The West;Esos</v>
+      </c>
+    </row>
+    <row r="44" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B44" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" t="s">
+        <v>42</v>
+      </c>
+      <c r="D44" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 7;Season 5</v>
+      </c>
+      <c r="F44" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" t="s">
+        <v>54</v>
+      </c>
+      <c r="H44" t="str">
+        <f>G44&amp;";"&amp;F44</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I44" t="s">
+        <v>56</v>
+      </c>
+      <c r="J44" t="str">
+        <f>I44&amp;";"&amp;H44</f>
+        <v>Qohor;The West;Esos</v>
+      </c>
+    </row>
+    <row r="45" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" t="s">
+        <v>43</v>
+      </c>
+      <c r="D45" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 8;Season 5</v>
+      </c>
+      <c r="F45" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" t="s">
+        <v>54</v>
+      </c>
+      <c r="H45" t="str">
+        <f>G45&amp;";"&amp;F45</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I45" t="s">
+        <v>57</v>
+      </c>
+      <c r="J45" t="str">
+        <f>I45&amp;";"&amp;H45</f>
+        <v>The Sorrow;The West;Esos</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46" t="s">
+        <v>35</v>
+      </c>
+      <c r="D46" t="str">
+        <f t="shared" si="0"/>
+        <v>Cahpter 9;Season 5</v>
+      </c>
+      <c r="F46" t="s">
+        <v>26</v>
+      </c>
+      <c r="G46" t="s">
+        <v>54</v>
+      </c>
+      <c r="H46" t="str">
+        <f>G46&amp;";"&amp;F46</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I46" t="s">
+        <v>58</v>
+      </c>
+      <c r="J46" t="str">
+        <f>I46&amp;";"&amp;H46</f>
+        <v>Mantarys;The West;Esos</v>
+      </c>
+    </row>
+    <row r="47" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C38" t="s">
-        <v>48</v>
-      </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 1;Season 5</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B39" t="s">
+      <c r="C47" t="s">
         <v>46</v>
       </c>
-      <c r="C39" t="s">
-        <v>49</v>
-      </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 2;Season 5</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B40" t="s">
-        <v>46</v>
-      </c>
-      <c r="C40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 3;Season 5</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" t="s">
-        <v>46</v>
-      </c>
-      <c r="C41" t="s">
-        <v>51</v>
-      </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 4;Season 5</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 5;Season 5</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" t="s">
-        <v>46</v>
-      </c>
-      <c r="C43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 6;Season 5</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" t="s">
-        <v>46</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="D47" t="str">
+        <f t="shared" si="0"/>
+        <v>Not in the show;Not in the show</v>
+      </c>
+      <c r="F47" t="s">
+        <v>26</v>
+      </c>
+      <c r="G47" t="s">
         <v>54</v>
       </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 7;Season 5</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B45" t="s">
-        <v>46</v>
-      </c>
-      <c r="C45" t="s">
-        <v>55</v>
-      </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 8;Season 5</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B46" t="s">
-        <v>46</v>
-      </c>
-      <c r="C46" t="s">
-        <v>47</v>
-      </c>
-      <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>Cahpter 9;Season 5</v>
-      </c>
-    </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B47" t="s">
-        <v>58</v>
-      </c>
-      <c r="C47" t="s">
-        <v>58</v>
-      </c>
-      <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>Not in the show;Not in the show</v>
+      <c r="H47" t="str">
+        <f>G47&amp;";"&amp;F47</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I47" t="s">
+        <v>59</v>
+      </c>
+      <c r="J47" t="str">
+        <f>I47&amp;";"&amp;H47</f>
+        <v>Astapor;The West;Esos</v>
+      </c>
+    </row>
+    <row r="48" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="F48" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" t="s">
+        <v>54</v>
+      </c>
+      <c r="H48" t="str">
+        <f>G48&amp;";"&amp;F48</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J48" t="str">
+        <f>I48&amp;";"&amp;H48</f>
+        <v>Vaes Dothrak;The West;Esos</v>
+      </c>
+    </row>
+    <row r="49" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F49" t="s">
+        <v>26</v>
+      </c>
+      <c r="G49" t="s">
+        <v>54</v>
+      </c>
+      <c r="H49" t="str">
+        <f>G49&amp;";"&amp;F49</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I49" t="s">
+        <v>61</v>
+      </c>
+      <c r="J49" t="str">
+        <f>I49&amp;";"&amp;H49</f>
+        <v>Yunkai;The West;Esos</v>
+      </c>
+    </row>
+    <row r="50" spans="6:10" x14ac:dyDescent="0.2">
+      <c r="F50" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" t="s">
+        <v>54</v>
+      </c>
+      <c r="H50" t="str">
+        <f>G50&amp;";"&amp;F50</f>
+        <v>The West;Esos</v>
+      </c>
+      <c r="I50" t="s">
+        <v>62</v>
+      </c>
+      <c r="J50" t="str">
+        <f>I50&amp;";"&amp;H50</f>
+        <v>Meereen;The West;Esos</v>
       </c>
     </row>
   </sheetData>

</xml_diff>